<commit_message>
csv changed brazil soy
</commit_message>
<xml_diff>
--- a/brazil-soy.xlsx
+++ b/brazil-soy.xlsx
@@ -635,8 +635,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -645,17 +646,15 @@
             <c:v>Deforestation in Hectares</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'brazil-soy'!$A$1:$A$14</c:f>
@@ -758,8 +757,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="145312720"/>
+        <c:axId val="145311152"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -890,12 +903,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="366996272"/>
-        <c:axId val="367001368"/>
+        <c:axId val="361027344"/>
+        <c:axId val="361025776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="366996272"/>
+        <c:axId val="145312720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -938,7 +952,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="367001368"/>
+        <c:crossAx val="145311152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -946,7 +960,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="367001368"/>
+        <c:axId val="145311152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -997,10 +1011,69 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="366996272"/>
+        <c:crossAx val="145312720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="361025776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="361027344"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="361027344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="361025776"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>

</xml_diff>